<commit_message>
updated BOM from digikey
</commit_message>
<xml_diff>
--- a/kicad/BOM_v02.xlsx
+++ b/kicad/BOM_v02.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="BOM_v02" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Bom_8266889" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
   <si>
     <t xml:space="preserve">Manufacturer Part Number</t>
   </si>
@@ -85,6 +85,9 @@
     <t xml:space="preserve">Active</t>
   </si>
   <si>
+    <t xml:space="preserve">$5.92</t>
+  </si>
+  <si>
     <t xml:space="preserve">12 Weeks</t>
   </si>
   <si>
@@ -112,6 +115,9 @@
     <t xml:space="preserve">Cut Tape (CT)</t>
   </si>
   <si>
+    <t xml:space="preserve">$0.66</t>
+  </si>
+  <si>
     <t xml:space="preserve">LED RED CLEAR 2PLCC SMD</t>
   </si>
   <si>
@@ -124,6 +130,9 @@
     <t xml:space="preserve">1497-1337-1-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">$0.74</t>
+  </si>
+  <si>
     <t xml:space="preserve">LED GREEN CLEAR 2PLCC</t>
   </si>
   <si>
@@ -133,6 +142,9 @@
     <t xml:space="preserve">1497-1334-1-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">$0.54</t>
+  </si>
+  <si>
     <t xml:space="preserve">LED YELLOW CLEAR 2PLCC SMD</t>
   </si>
   <si>
@@ -145,6 +157,9 @@
     <t xml:space="preserve">311-330FRCT-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">$0.50</t>
+  </si>
+  <si>
     <t xml:space="preserve">24 Weeks</t>
   </si>
   <si>
@@ -160,70 +175,85 @@
     <t xml:space="preserve">ATTINY85-20SURCT-ND</t>
   </si>
   <si>
+    <t xml:space="preserve">$1.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17 Weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IC MCU 8BIT 8KB FLASH 8SOIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keystone Electronics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36-3034-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bulk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$0.31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 Weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BATTERY RETAINER COIN 20MM SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN-S124ARUW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inolux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1830-1119-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$0.82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED WHITE CLEAR 1204 SMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SR99S01VBNN00G7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METZ CONNECT USA Inc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1849-1167-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$2.32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 Weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TERM BLOCK 1POS SIDE ENTRY PCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RoHS Compliant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JS202011SCQN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C&amp;K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">401-2002-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$0.60</t>
+  </si>
+  <si>
     <t xml:space="preserve">13 Weeks</t>
   </si>
   <si>
-    <t xml:space="preserve">IC MCU 8BIT 8KB FLASH 8SOIC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keystone Electronics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36-3034-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bulk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6 Weeks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BATTERY RETAINER COIN 20MM SMD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN-S124ARUW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inolux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1830-1119-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED WHITE CLEAR 1204 SMD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SR99S01VBNN00G7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">METZ CONNECT USA Inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1849-1167-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 Weeks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TERM BLOCK 1POS SIDE ENTRY PCB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RoHS Compliant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JS202011SCQN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C&amp;K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">401-2002-1-ND</t>
-  </si>
-  <si>
     <t xml:space="preserve">SWITCH SLIDE DPDT 300MA 6V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total</t>
   </si>
 </sst>
 </file>
@@ -232,7 +262,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -303,18 +333,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -324,15 +354,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.11"/>
@@ -344,11 +374,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="35.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="35.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="16.99"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -423,41 +452,40 @@
       <c r="I2" s="0" t="n">
         <v>2.96</v>
       </c>
-      <c r="J2" s="1" t="n">
-        <f aca="false">H2*I2</f>
-        <v>5.92</v>
+      <c r="J2" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>3206</v>
+        <v>3094</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>20</v>
@@ -468,41 +496,40 @@
       <c r="I3" s="0" t="n">
         <v>0.66</v>
       </c>
-      <c r="J3" s="1" t="n">
-        <f aca="false">H3*I3</f>
-        <v>0.66</v>
+      <c r="J3" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>0</v>
+        <v>1772</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>20</v>
@@ -513,41 +540,40 @@
       <c r="I4" s="0" t="n">
         <v>0.74</v>
       </c>
-      <c r="J4" s="1" t="n">
-        <f aca="false">H4*I4</f>
-        <v>0.74</v>
+      <c r="J4" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>98809</v>
+        <v>98154</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>20</v>
@@ -558,41 +584,40 @@
       <c r="I5" s="0" t="n">
         <v>0.54</v>
       </c>
-      <c r="J5" s="1" t="n">
-        <f aca="false">H5*I5</f>
-        <v>0.54</v>
+      <c r="J5" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>21248</v>
+        <v>21238</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>20</v>
@@ -603,41 +628,40 @@
       <c r="I6" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="J6" s="1" t="n">
-        <f aca="false">H6*I6</f>
-        <v>0.5</v>
+      <c r="J6" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="K6" s="0" t="n">
-        <v>49548</v>
+        <v>31990</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>20</v>
@@ -648,27 +672,26 @@
       <c r="I7" s="0" t="n">
         <v>1.19</v>
       </c>
-      <c r="J7" s="1" t="n">
-        <f aca="false">H7*I7</f>
-        <v>1.19</v>
+      <c r="J7" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>9808</v>
+        <v>8552</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,13 +699,13 @@
         <v>3034</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>20</v>
@@ -693,41 +716,40 @@
       <c r="I8" s="0" t="n">
         <v>0.31</v>
       </c>
-      <c r="J8" s="1" t="n">
-        <f aca="false">H8*I8</f>
-        <v>0.31</v>
+      <c r="J8" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="K8" s="0" t="n">
-        <v>28716</v>
+        <v>5529</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>20</v>
@@ -738,41 +760,40 @@
       <c r="I9" s="0" t="n">
         <v>0.41</v>
       </c>
-      <c r="J9" s="1" t="n">
-        <f aca="false">H9*I9</f>
-        <v>0.82</v>
+      <c r="J9" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="K9" s="0" t="n">
-        <v>54525</v>
+        <v>17759</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>20</v>
@@ -783,41 +804,40 @@
       <c r="I10" s="0" t="n">
         <v>1.16</v>
       </c>
-      <c r="J10" s="1" t="n">
-        <f aca="false">H10*I10</f>
-        <v>2.32</v>
+      <c r="J10" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="K10" s="0" t="n">
-        <v>4646</v>
+        <v>6098</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>20</v>
@@ -828,39 +848,26 @@
       <c r="I11" s="0" t="n">
         <v>0.6</v>
       </c>
-      <c r="J11" s="1" t="n">
-        <f aca="false">H11*I11</f>
-        <v>0.6</v>
+      <c r="J11" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="K11" s="0" t="n">
-        <v>34730</v>
+        <v>30511</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I13" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="J13" s="1" t="n">
-        <f aca="false">SUM(J2:J11)</f>
-        <v>13.6</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>